<commit_message>
Common Setup For Provisioning Class and Removing the Portfolio Excel
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/ExamCenterDetails.xlsx
+++ b/src/test/resources/ExcelFiles/ExamCenterDetails.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Focalpoint Automation\FPK12AutomationProject\src\test\resources\ExcelFiles\"/>
     </mc:Choice>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="58">
   <si>
     <t>Location</t>
   </si>
@@ -152,12 +152,73 @@
   </si>
   <si>
     <t>ECLocation65237</t>
+  </si>
+  <si>
+    <t>ECLocation20711</t>
+  </si>
+  <si>
+    <t>48482</t>
+  </si>
+  <si>
+    <t>86768</t>
+  </si>
+  <si>
+    <t>54190</t>
+  </si>
+  <si>
+    <t>FPK12Exam48625</t>
+  </si>
+  <si>
+    <t>FPK12Schedule87107</t>
+  </si>
+  <si>
+    <t>ECLocation98261</t>
+  </si>
+  <si>
+    <t>ECLocation56395</t>
+  </si>
+  <si>
+    <t>21233</t>
+  </si>
+  <si>
+    <t>22417</t>
+  </si>
+  <si>
+    <t>56631</t>
+  </si>
+  <si>
+    <t>FPK12Exam89648</t>
+  </si>
+  <si>
+    <t>FPK12Schedule34284</t>
+  </si>
+  <si>
+    <t>ECLocation18037</t>
+  </si>
+  <si>
+    <t>ECLocation85039</t>
+  </si>
+  <si>
+    <t>90268</t>
+  </si>
+  <si>
+    <t>67503</t>
+  </si>
+  <si>
+    <t>13296</t>
+  </si>
+  <si>
+    <t>FPK12Exam65780</t>
+  </si>
+  <si>
+    <t>FPK12Schedule95731</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -242,7 +303,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -287,11 +348,18 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <right style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -346,6 +414,39 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -688,15 +789,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.21875" customWidth="1"/>
-    <col min="2" max="2" width="21.77734375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="18.44140625" style="11" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" customWidth="1"/>
-    <col min="5" max="5" width="20" style="11" customWidth="1"/>
-    <col min="6" max="6" width="28.5546875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="12.5546875" customWidth="1"/>
-    <col min="8" max="8" width="18.88671875" customWidth="1"/>
-    <col min="9" max="9" width="23.109375" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="17.21875"/>
+    <col min="2" max="2" customWidth="true" style="3" width="21.77734375"/>
+    <col min="3" max="3" customWidth="true" style="11" width="18.44140625"/>
+    <col min="4" max="4" customWidth="true" width="14.88671875"/>
+    <col min="5" max="5" customWidth="true" style="11" width="20.0"/>
+    <col min="6" max="6" customWidth="true" style="3" width="28.5546875"/>
+    <col min="7" max="7" customWidth="true" width="12.5546875"/>
+    <col min="8" max="8" customWidth="true" width="18.88671875"/>
+    <col min="9" max="9" customWidth="true" width="23.109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -729,8 +830,8 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
-        <v>37</v>
+      <c r="A2" t="s" s="28">
+        <v>52</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>16</v>
@@ -748,11 +849,11 @@
       <c r="G2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="I2" s="19" t="s">
-        <v>36</v>
+      <c r="H2" t="s" s="29">
+        <v>56</v>
+      </c>
+      <c r="I2" t="s" s="30">
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -765,7 +866,7 @@
         <v>13</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="F3" s="5">
         <v>1367</v>
@@ -786,7 +887,7 @@
         <v>14</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="F4" s="5">
         <v>1367</v>
@@ -807,7 +908,7 @@
         <v>15</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="F5" s="5">
         <v>1367</v>
@@ -833,15 +934,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.21875" customWidth="1"/>
-    <col min="2" max="2" width="21.77734375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="18.44140625" style="11" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" customWidth="1"/>
-    <col min="5" max="5" width="20" style="11" customWidth="1"/>
-    <col min="6" max="6" width="28.5546875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="12.5546875" customWidth="1"/>
-    <col min="8" max="8" width="18.88671875" customWidth="1"/>
-    <col min="9" max="9" width="23.109375" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="17.21875"/>
+    <col min="2" max="2" customWidth="true" style="3" width="21.77734375"/>
+    <col min="3" max="3" customWidth="true" style="11" width="18.44140625"/>
+    <col min="4" max="4" customWidth="true" width="14.88671875"/>
+    <col min="5" max="5" customWidth="true" style="11" width="20.0"/>
+    <col min="6" max="6" customWidth="true" style="3" width="28.5546875"/>
+    <col min="7" max="7" customWidth="true" width="12.5546875"/>
+    <col min="8" max="8" customWidth="true" width="18.88671875"/>
+    <col min="9" max="9" customWidth="true" width="23.109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -978,14 +1079,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" customWidth="1"/>
-    <col min="4" max="5" width="17.109375" customWidth="1"/>
-    <col min="6" max="6" width="11.77734375" customWidth="1"/>
-    <col min="7" max="7" width="15.5546875" customWidth="1"/>
-    <col min="8" max="8" width="16" customWidth="1"/>
-    <col min="9" max="9" width="22.44140625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="18.6640625"/>
+    <col min="2" max="2" customWidth="true" width="20.0"/>
+    <col min="3" max="3" customWidth="true" width="12.6640625"/>
+    <col min="4" max="5" customWidth="true" width="17.109375"/>
+    <col min="6" max="6" customWidth="true" width="11.77734375"/>
+    <col min="7" max="7" customWidth="true" width="15.5546875"/>
+    <col min="8" max="8" customWidth="true" width="16.0"/>
+    <col min="9" max="9" customWidth="true" width="22.44140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -1025,7 +1126,7 @@
         <v>16</v>
       </c>
       <c r="C2" s="12"/>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>8</v>
       </c>
       <c r="E2" s="14" t="s">

</xml_diff>

<commit_message>
Latest Code & Handled Stale Element reference Exception
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/ExamCenterDetails.xlsx
+++ b/src/test/resources/ExcelFiles/ExamCenterDetails.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="143">
   <si>
     <t>Location</t>
   </si>
@@ -431,6 +431,42 @@
   </si>
   <si>
     <t>FPK12Exam66911</t>
+  </si>
+  <si>
+    <t>ECLocation29852</t>
+  </si>
+  <si>
+    <t>1358</t>
+  </si>
+  <si>
+    <t>44670</t>
+  </si>
+  <si>
+    <t>11766</t>
+  </si>
+  <si>
+    <t>FPK12Exam28220</t>
+  </si>
+  <si>
+    <t>FPK12Schedule42629</t>
+  </si>
+  <si>
+    <t>ECLocation50954</t>
+  </si>
+  <si>
+    <t>45044</t>
+  </si>
+  <si>
+    <t>59184</t>
+  </si>
+  <si>
+    <t>42692</t>
+  </si>
+  <si>
+    <t>FPK12Exam53770</t>
+  </si>
+  <si>
+    <t>FPK12Schedule28586</t>
   </si>
 </sst>
 </file>
@@ -578,7 +614,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -633,6 +669,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
       <alignment vertical="center" horizontal="center"/>
     </xf>
@@ -1169,8 +1223,8 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="69">
-        <v>129</v>
+      <c r="A2" t="s" s="74">
+        <v>137</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>16</v>
@@ -1188,11 +1242,11 @@
       <c r="G2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H2" t="s" s="70">
-        <v>130</v>
-      </c>
-      <c r="I2" t="s" s="67">
-        <v>127</v>
+      <c r="H2" t="s" s="75">
+        <v>141</v>
+      </c>
+      <c r="I2" t="s" s="76">
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -1205,7 +1259,7 @@
         <v>13</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>123</v>
+        <v>138</v>
       </c>
       <c r="F3" s="5">
         <v>1367</v>
@@ -1226,7 +1280,7 @@
         <v>14</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>124</v>
+        <v>139</v>
       </c>
       <c r="F4" s="5">
         <v>1367</v>
@@ -1247,7 +1301,7 @@
         <v>15</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="F5" s="5">
         <v>1367</v>

</xml_diff>

<commit_message>
Latest Updated Script for Parallel Execution
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/ExamCenterDetails.xlsx
+++ b/src/test/resources/ExcelFiles/ExamCenterDetails.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="186">
   <si>
     <t>Location</t>
   </si>
@@ -467,6 +467,135 @@
   </si>
   <si>
     <t>FPK12Schedule28586</t>
+  </si>
+  <si>
+    <t>ECLocation83209</t>
+  </si>
+  <si>
+    <t>37618</t>
+  </si>
+  <si>
+    <t>51790</t>
+  </si>
+  <si>
+    <t>30122</t>
+  </si>
+  <si>
+    <t>FPK12Exam99639</t>
+  </si>
+  <si>
+    <t>FPK12Schedule17160</t>
+  </si>
+  <si>
+    <t>ECLocation63971</t>
+  </si>
+  <si>
+    <t>27653</t>
+  </si>
+  <si>
+    <t>63269</t>
+  </si>
+  <si>
+    <t>97770</t>
+  </si>
+  <si>
+    <t>FPK12Exam39839</t>
+  </si>
+  <si>
+    <t>FPK12Schedule4162</t>
+  </si>
+  <si>
+    <t>ECLocation88388</t>
+  </si>
+  <si>
+    <t>ECLocation80637</t>
+  </si>
+  <si>
+    <t>ECLocation61023</t>
+  </si>
+  <si>
+    <t>ECLocation52228</t>
+  </si>
+  <si>
+    <t>ECLocation26455</t>
+  </si>
+  <si>
+    <t>54179</t>
+  </si>
+  <si>
+    <t>10923</t>
+  </si>
+  <si>
+    <t>61803</t>
+  </si>
+  <si>
+    <t>FPK12Exam82222</t>
+  </si>
+  <si>
+    <t>FPK12Schedule53346</t>
+  </si>
+  <si>
+    <t>ECLocation12234</t>
+  </si>
+  <si>
+    <t>ECLocation16568</t>
+  </si>
+  <si>
+    <t>71779</t>
+  </si>
+  <si>
+    <t>59760</t>
+  </si>
+  <si>
+    <t>69627</t>
+  </si>
+  <si>
+    <t>FPK12Exam82748</t>
+  </si>
+  <si>
+    <t>FPK12Schedule58910</t>
+  </si>
+  <si>
+    <t>ECLocation53720</t>
+  </si>
+  <si>
+    <t>69518</t>
+  </si>
+  <si>
+    <t>89108</t>
+  </si>
+  <si>
+    <t>15076</t>
+  </si>
+  <si>
+    <t>FPK12Exam78459</t>
+  </si>
+  <si>
+    <t>FPK12Schedule1684</t>
+  </si>
+  <si>
+    <t>ECLocation10372</t>
+  </si>
+  <si>
+    <t>FPK12Exam55404</t>
+  </si>
+  <si>
+    <t>ECLocation21953</t>
+  </si>
+  <si>
+    <t>87737</t>
+  </si>
+  <si>
+    <t>87927</t>
+  </si>
+  <si>
+    <t>37737</t>
+  </si>
+  <si>
+    <t>FPK12Exam38575</t>
+  </si>
+  <si>
+    <t>FPK12Schedule10282</t>
   </si>
 </sst>
 </file>
@@ -614,7 +743,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -669,6 +798,81 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
       <alignment vertical="center" horizontal="center"/>
     </xf>
@@ -1223,8 +1427,8 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="74">
-        <v>137</v>
+      <c r="A2" t="s" s="99">
+        <v>180</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>16</v>
@@ -1242,11 +1446,11 @@
       <c r="G2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H2" t="s" s="75">
-        <v>141</v>
-      </c>
-      <c r="I2" t="s" s="76">
-        <v>142</v>
+      <c r="H2" t="s" s="100">
+        <v>184</v>
+      </c>
+      <c r="I2" t="s" s="101">
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -1259,7 +1463,7 @@
         <v>13</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>138</v>
+        <v>181</v>
       </c>
       <c r="F3" s="5">
         <v>1367</v>
@@ -1280,7 +1484,7 @@
         <v>14</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>139</v>
+        <v>182</v>
       </c>
       <c r="F4" s="5">
         <v>1367</v>
@@ -1301,7 +1505,7 @@
         <v>15</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>140</v>
+        <v>183</v>
       </c>
       <c r="F5" s="5">
         <v>1367</v>

</xml_diff>

<commit_message>
Latest Updated Script with xpaths Changes
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/ExamCenterDetails.xlsx
+++ b/src/test/resources/ExcelFiles/ExamCenterDetails.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="74">
   <si>
     <t>Location</t>
   </si>
@@ -257,6 +257,9 @@
   </si>
   <si>
     <t>FPK12Schedule65257</t>
+  </si>
+  <si>
+    <t>ECLocation4867</t>
   </si>
 </sst>
 </file>
@@ -409,7 +412,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -465,6 +468,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
       <alignment vertical="center" horizontal="center"/>
@@ -906,8 +912,8 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="36">
-        <v>67</v>
+      <c r="A2" t="s" s="39">
+        <v>73</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
Initial commit - uploaded automation project
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/ExamCenterDetails.xlsx
+++ b/src/test/resources/ExcelFiles/ExamCenterDetails.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Focalpoint Automation\FPK12AutomationProject\src\test\resources\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E94872-D1DF-4371-A994-E3334611A1E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{216F39F0-AB53-46AE-9FD1-662DCB99E2F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{59011258-3E7A-408E-B881-47367FDC8FB6}"/>
+    <workbookView xWindow="4212" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{59011258-3E7A-408E-B881-47367FDC8FB6}"/>
   </bookViews>
   <sheets>
     <sheet name="STAGE" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="57">
   <si>
     <t>Location</t>
   </si>
@@ -94,24 +94,6 @@
     <t>testexam</t>
   </si>
   <si>
-    <t>ECLocation89622</t>
-  </si>
-  <si>
-    <t>61845</t>
-  </si>
-  <si>
-    <t>96085</t>
-  </si>
-  <si>
-    <t>83116</t>
-  </si>
-  <si>
-    <t>FPK12Exam74398</t>
-  </si>
-  <si>
-    <t>FPK12Schedule21348</t>
-  </si>
-  <si>
     <t>fpadminqa</t>
   </si>
   <si>
@@ -136,130 +118,97 @@
     <t>admin</t>
   </si>
   <si>
-    <t>ECLocation91322</t>
-  </si>
-  <si>
-    <t>3036</t>
-  </si>
-  <si>
-    <t>37405</t>
-  </si>
-  <si>
-    <t>95779</t>
-  </si>
-  <si>
-    <t>FPK12Exam48206</t>
-  </si>
-  <si>
-    <t>FPK12Schedule30646</t>
-  </si>
-  <si>
     <t>FPK12 Automation Test</t>
   </si>
   <si>
-    <t>ECLocation3844</t>
-  </si>
-  <si>
-    <t>33284</t>
-  </si>
-  <si>
-    <t>52580</t>
-  </si>
-  <si>
-    <t>61217</t>
-  </si>
-  <si>
-    <t>FPK12Exam9536</t>
-  </si>
-  <si>
-    <t>FPK12Schedule1135</t>
-  </si>
-  <si>
-    <t>ECLocation90107</t>
-  </si>
-  <si>
-    <t>15684</t>
-  </si>
-  <si>
-    <t>49620</t>
-  </si>
-  <si>
-    <t>11283</t>
-  </si>
-  <si>
-    <t>FPK12Exam2985</t>
-  </si>
-  <si>
-    <t>FPK12Schedule89212</t>
-  </si>
-  <si>
-    <t>ECLocation58322</t>
-  </si>
-  <si>
-    <t>20497</t>
-  </si>
-  <si>
-    <t>69011</t>
-  </si>
-  <si>
-    <t>95346</t>
-  </si>
-  <si>
-    <t>ECLocation55574</t>
-  </si>
-  <si>
-    <t>8464</t>
-  </si>
-  <si>
-    <t>96628</t>
-  </si>
-  <si>
-    <t>84645</t>
-  </si>
-  <si>
-    <t>FPK12Exam53617</t>
-  </si>
-  <si>
-    <t>FPK12Schedule13202</t>
-  </si>
-  <si>
-    <t>ECLocation30599</t>
-  </si>
-  <si>
-    <t>FPK12Exam29110</t>
-  </si>
-  <si>
-    <t>FPK12Schedule58281</t>
-  </si>
-  <si>
-    <t>ECLocation13492</t>
-  </si>
-  <si>
-    <t>FPK12Exam45739</t>
-  </si>
-  <si>
-    <t>FPK12Schedule14150</t>
-  </si>
-  <si>
-    <t>ECLocation70692</t>
-  </si>
-  <si>
-    <t>76114</t>
-  </si>
-  <si>
-    <t>19809</t>
-  </si>
-  <si>
-    <t>48676</t>
-  </si>
-  <si>
-    <t>FPK12Exam85267</t>
-  </si>
-  <si>
-    <t>FPK12Schedule65257</t>
-  </si>
-  <si>
-    <t>ECLocation4867</t>
+    <t>ECLocation84969</t>
+  </si>
+  <si>
+    <t>36066</t>
+  </si>
+  <si>
+    <t>90881</t>
+  </si>
+  <si>
+    <t>90672</t>
+  </si>
+  <si>
+    <t>FPK12Exam95142</t>
+  </si>
+  <si>
+    <t>FPK12Schedule84993</t>
+  </si>
+  <si>
+    <t>FPK12Schedule42107</t>
+  </si>
+  <si>
+    <t>ECLocation15958</t>
+  </si>
+  <si>
+    <t>68595</t>
+  </si>
+  <si>
+    <t>44508</t>
+  </si>
+  <si>
+    <t>47001</t>
+  </si>
+  <si>
+    <t>FPK12Exam68888</t>
+  </si>
+  <si>
+    <t>ECLocation85771</t>
+  </si>
+  <si>
+    <t>FPK12Exam82400</t>
+  </si>
+  <si>
+    <t>FPK12Schedule47023</t>
+  </si>
+  <si>
+    <t>ECLocation99139</t>
+  </si>
+  <si>
+    <t>ECLocation37347</t>
+  </si>
+  <si>
+    <t>ECLocation5282</t>
+  </si>
+  <si>
+    <t>ECLocation70980</t>
+  </si>
+  <si>
+    <t>19556</t>
+  </si>
+  <si>
+    <t>96067</t>
+  </si>
+  <si>
+    <t>69906</t>
+  </si>
+  <si>
+    <t>FPK12Exam26482</t>
+  </si>
+  <si>
+    <t>FPK12Schedule9078</t>
+  </si>
+  <si>
+    <t>ECLocation87635</t>
+  </si>
+  <si>
+    <t>62598</t>
+  </si>
+  <si>
+    <t>11507</t>
+  </si>
+  <si>
+    <t>81993</t>
+  </si>
+  <si>
+    <t>FPK12Exam65831</t>
+  </si>
+  <si>
+    <t>FPK12Schedule54736</t>
   </si>
 </sst>
 </file>
@@ -345,7 +294,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -391,17 +340,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <bottom style="thin"/>
     </border>
     <border>
@@ -412,7 +350,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -466,67 +404,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
       <alignment vertical="center" horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
       <alignment vertical="center" horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
       <alignment vertical="center" horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
       <alignment vertical="center" horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
       <alignment vertical="center" horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
       <alignment vertical="center" horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
       <alignment vertical="center" horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
       <alignment vertical="center" horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
       <alignment vertical="center" horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
       <alignment vertical="center" horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
       <alignment vertical="center" horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
       <alignment vertical="center" horizontal="center"/>
     </xf>
   </cellXfs>
@@ -912,15 +823,15 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="39">
-        <v>73</v>
+      <c r="A2" t="s" s="28">
+        <v>51</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="9" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E2" s="14" t="s">
         <v>8</v>
@@ -931,11 +842,11 @@
       <c r="G2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H2" t="s" s="37">
-        <v>71</v>
-      </c>
-      <c r="I2" t="s" s="38">
-        <v>72</v>
+      <c r="H2" t="s" s="29">
+        <v>55</v>
+      </c>
+      <c r="I2" t="s" s="30">
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -948,7 +859,7 @@
         <v>13</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="F3" s="5">
         <v>1367</v>
@@ -969,7 +880,7 @@
         <v>14</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="F4" s="5">
         <v>1367</v>
@@ -990,7 +901,7 @@
         <v>15</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="F5" s="5">
         <v>1367</v>
@@ -1057,8 +968,8 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
-        <v>18</v>
+      <c r="A2" s="18" t="s">
+        <v>27</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>16</v>
@@ -1076,11 +987,11 @@
       <c r="G2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="17" t="s">
-        <v>23</v>
+      <c r="H2" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -1093,7 +1004,7 @@
         <v>13</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="F3" s="5">
         <v>2</v>
@@ -1114,7 +1025,7 @@
         <v>14</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="F4" s="5">
         <v>2</v>
@@ -1135,7 +1046,7 @@
         <v>15</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="F5" s="5">
         <v>2</v>
@@ -1201,8 +1112,8 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
-        <v>25</v>
+      <c r="A2" s="17" t="s">
+        <v>19</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>16</v>
@@ -1212,7 +1123,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F2" s="5">
         <v>250</v>
@@ -1220,11 +1131,11 @@
       <c r="G2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="I2" s="18" t="s">
-        <v>30</v>
+      <c r="H2" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -1237,7 +1148,7 @@
         <v>13</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="F3" s="5">
         <v>250</v>
@@ -1258,7 +1169,7 @@
         <v>14</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F4" s="5">
         <v>250</v>
@@ -1279,7 +1190,7 @@
         <v>15</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F5" s="5">
         <v>250</v>

</xml_diff>